<commit_message>
Affiliation video and records
</commit_message>
<xml_diff>
--- a/public/downloads/eu-records/TESTED-FP-RAW.xlsx
+++ b/public/downloads/eu-records/TESTED-FP-RAW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b791772ed41bd66b/Desktop/COMONWELTH ^0 EUROPEN RECORDES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1611" documentId="8_{406763AE-22C8-4994-A1E8-52D3B1C82B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A71602A-D943-4129-8434-7625A9C2AE43}"/>
+  <xr:revisionPtr revIDLastSave="1649" documentId="8_{406763AE-22C8-4994-A1E8-52D3B1C82B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9E14BC6-AF41-4FF2-8ACA-009762CD317D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{4154235A-A9CC-3C49-98D1-D24EB0BE76D8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4154235A-A9CC-3C49-98D1-D24EB0BE76D8}"/>
   </bookViews>
   <sheets>
     <sheet name="MEN OPEN" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="155">
   <si>
     <t>Weight</t>
   </si>
@@ -477,6 +477,36 @@
   <si>
     <t>640.0KG</t>
   </si>
+  <si>
+    <t>VASILE BUCEAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORD BRAKERS </t>
+  </si>
+  <si>
+    <t>510.0KG</t>
+  </si>
+  <si>
+    <t>ROUMANIA</t>
+  </si>
+  <si>
+    <t>GHEORGHE BUCEAC</t>
+  </si>
+  <si>
+    <t>RECORD BRAKERS</t>
+  </si>
+  <si>
+    <t>310.0KG</t>
+  </si>
+  <si>
+    <t>185.0KG</t>
+  </si>
+  <si>
+    <t>300.0KG</t>
+  </si>
+  <si>
+    <t>795.0KG</t>
+  </si>
 </sst>
 </file>
 
@@ -901,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306999F4-8918-254E-B53D-F64ABC5BF343}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1308,7 +1338,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>13</v>
@@ -1316,45 +1346,89 @@
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D35" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1363,7 +1437,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>14</v>
@@ -1376,7 +1450,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
@@ -1387,7 +1461,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
@@ -1398,7 +1472,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
@@ -1409,7 +1483,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1418,7 +1492,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>15</v>
@@ -1431,7 +1505,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -1442,7 +1516,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
@@ -1453,7 +1527,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
@@ -1464,7 +1538,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1473,7 +1547,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="1" t="s">
         <v>16</v>
@@ -1481,10 +1555,21 @@
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
@@ -1492,10 +1577,21 @@
       <c r="C49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E49" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
@@ -1503,10 +1599,21 @@
       <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
@@ -1514,10 +1621,21 @@
       <c r="C51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E51" s="13">
+        <v>45256</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H51" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
@@ -2935,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68180E9-570C-BE40-A2EC-46381CEBEE35}">
   <dimension ref="A1:I556"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B236" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G243" sqref="F243:G248"/>
+    <sheetView topLeftCell="B236" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E238" sqref="E238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>